<commit_message>
fixed after Avi's comments
</commit_message>
<xml_diff>
--- a/Docs/requirements traceability.xlsx
+++ b/Docs/requirements traceability.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F97333-7ADE-4CF7-98C0-D161E6F723EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E29E114B-0B5D-48F1-BBAE-137E75C3EF64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36600" yWindow="1035" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,9 +433,6 @@
 RemovePermissionPermissionTest</t>
   </si>
   <si>
-    <t>יש להשלים allowManagerToGetHistory</t>
-  </si>
-  <si>
     <t>בעל-חנות רשאי להסיר מינוי של מנהל-חנות שמונה על ידו בעבר</t>
   </si>
   <si>
@@ -469,19 +466,22 @@
     <t>same as 4.6</t>
   </si>
   <si>
-    <t>יש תשתית לפניה. מע' תשלומים לא קיימת</t>
-  </si>
-  <si>
     <t>PaymentSystem.pay</t>
   </si>
   <si>
     <t>DeliverySystem.deliver</t>
   </si>
   <si>
-    <t>יש תשתית לפניה. מע' אספקה לא קיימת</t>
-  </si>
-  <si>
     <t>יש לממש ErrorLog ולהשלים בדיקות יחידה. יש להרחיב את בדיקות הקבלה ל- logs</t>
+  </si>
+  <si>
+    <t>יש תשתית לפניה. להוסיף mock למע' התשלומים בבדיקות הקבלה</t>
+  </si>
+  <si>
+    <t>יש תשתית לפניה. להוסיף mock למע' האספקה בבדיקות הקבלה</t>
+  </si>
+  <si>
+    <t>להוסיף טסטים</t>
   </si>
 </sst>
 </file>
@@ -599,29 +599,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,16 +915,16 @@
     <col min="2" max="2" width="9.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="60.88671875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="31.88671875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.33203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="60.88671875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="15" customWidth="1"/>
     <col min="9" max="9" width="34.21875" style="3" customWidth="1"/>
     <col min="10" max="12" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -939,21 +939,21 @@
       <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="6">
@@ -965,16 +965,16 @@
       <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I2" s="7" t="s">
@@ -982,7 +982,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="6">
@@ -994,22 +994,22 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>94</v>
       </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="6">
         <v>2.2000000000000002</v>
       </c>
@@ -1019,12 +1019,12 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="17" t="s">
+      <c r="E4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="16" t="s">
         <v>94</v>
       </c>
       <c r="I4" s="7" t="s">
@@ -1032,7 +1032,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="6">
         <v>2.2999999999999998</v>
       </c>
@@ -1042,22 +1042,22 @@
       <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>94</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="6">
         <v>2.4</v>
       </c>
@@ -1067,22 +1067,22 @@
       <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>94</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="6">
         <v>2.5</v>
       </c>
@@ -1092,22 +1092,22 @@
       <c r="D7" s="6">
         <v>1</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="6">
         <v>2.6</v>
       </c>
@@ -1117,22 +1117,22 @@
       <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>95</v>
       </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="6">
         <v>2.7</v>
       </c>
@@ -1142,22 +1142,22 @@
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="15" t="s">
+      <c r="E9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>96</v>
       </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6">
         <v>2.8</v>
       </c>
@@ -1167,22 +1167,22 @@
       <c r="D10" s="6">
         <v>1</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>96</v>
       </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6">
         <v>2.9</v>
       </c>
@@ -1192,14 +1192,14 @@
       <c r="D11" s="6">
         <v>1</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I11" s="7" t="s">
@@ -1207,7 +1207,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="6">
@@ -1219,22 +1219,22 @@
       <c r="D12" s="6">
         <v>1</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="15" t="s">
+      <c r="E12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>94</v>
       </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="6">
         <v>3.2</v>
       </c>
@@ -1244,22 +1244,22 @@
       <c r="D13" s="6">
         <v>1</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="15" t="s">
+      <c r="E13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="16" t="s">
         <v>94</v>
       </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="6">
         <v>3.3</v>
       </c>
@@ -1269,16 +1269,16 @@
       <c r="D14" s="6">
         <v>1</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -1286,7 +1286,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="6">
         <v>3.7</v>
       </c>
@@ -1296,16 +1296,16 @@
       <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I15" s="7" t="s">
@@ -1313,7 +1313,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="144" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="6">
@@ -1325,22 +1325,22 @@
       <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="17" t="s">
+      <c r="E16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="16" t="s">
         <v>99</v>
       </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="6">
         <v>4.3</v>
       </c>
@@ -1350,22 +1350,22 @@
       <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="16" t="s">
         <v>100</v>
       </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
@@ -1375,22 +1375,22 @@
       <c r="D18" s="6">
         <v>1</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="16" t="s">
         <v>102</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6">
         <v>4.5</v>
       </c>
@@ -1400,22 +1400,22 @@
       <c r="D19" s="6">
         <v>1</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="16" t="s">
         <v>103</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="6">
         <v>4.5999999999999996</v>
       </c>
@@ -1426,73 +1426,71 @@
         <v>1</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="H20" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="6">
         <v>4.7</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>106</v>
-      </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="6">
         <v>4.9000000000000004</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="6">
-        <v>1</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>109</v>
-      </c>
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="6">
         <v>4.1100000000000003</v>
       </c>
@@ -1502,24 +1500,24 @@
       <c r="D23" s="6">
         <v>1</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>110</v>
+      <c r="H23" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="6">
@@ -1531,22 +1529,22 @@
       <c r="D24" s="6">
         <v>1</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>111</v>
+      <c r="E24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="6">
@@ -1558,24 +1556,24 @@
       <c r="D25" s="6">
         <v>1</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>110</v>
+      <c r="H25" s="16" t="s">
+        <v>109</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="6">
@@ -1587,22 +1585,22 @@
       <c r="D26" s="6">
         <v>1</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15" t="s">
+      <c r="E26" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="6">
@@ -1614,14 +1612,14 @@
       <c r="D27" s="6">
         <v>1</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15" t="s">
+      <c r="E27" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I27" s="7" t="s">
@@ -1629,7 +1627,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="6">
@@ -1641,18 +1639,18 @@
       <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15" t="s">
+      <c r="E28" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="8" t="s">
         <v>30</v>
       </c>
@@ -1665,15 +1663,15 @@
       <c r="E29" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15" t="s">
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="6">
         <v>4</v>
       </c>
@@ -1683,18 +1681,20 @@
       <c r="D30" s="6">
         <v>1</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15" t="s">
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="7"/>
+      <c r="I30" s="7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="6">
         <v>7</v>
       </c>
@@ -1704,20 +1704,20 @@
       <c r="D31" s="6">
         <v>1</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="H31" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
requirements traceability updated for V2
</commit_message>
<xml_diff>
--- a/Docs/requirements traceability.xlsx
+++ b/Docs/requirements traceability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omrig\Desktop\BGU\semesterD\Workshop on Software Engineering Project\version2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E29E114B-0B5D-48F1-BBAE-137E75C3EF64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EF8DB7-5BED-4444-B4B7-BE037720ED37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36600" yWindow="1035" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="140">
   <si>
     <t>מס' דרישה</t>
   </si>
@@ -302,15 +302,238 @@
 wrongAppointStoreManager()</t>
   </si>
   <si>
-    <t>TradingSystemServiceImpl.allowManagerToUpdateProducts
+    <t>TradingSystemServiceImpl.removeManager</t>
+  </si>
+  <si>
+    <t>validRemoveManager()
+wrongRemoveManager()</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.showStaffInfo</t>
+  </si>
+  <si>
+    <t>showStaffInfo()
+showStaffInfoStoreNotExist()
+showStaffInfoNoPermissions()</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.getSalesHistoryByStore</t>
+  </si>
+  <si>
+    <t>getSalesHistoryByStore()
+wrongGetSalesHistoryByStore()</t>
+  </si>
+  <si>
+    <t>ביצוע תשלום</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.purchaseCart</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.getEventLog
+TradingSystemServiceImpl.getErrorLog</t>
+  </si>
+  <si>
+    <t>getEventLog()
+wrongGetEventLog()
+getErrorLog()
+wrongGetErrorLog()</t>
+  </si>
+  <si>
+    <t>בביצוע</t>
+  </si>
+  <si>
+    <t>אתחול המערכת המבטיח קיום כל הישויות הנדרשות על פי אילוצי הנכונות (למשל מערכת המסחר, מערכת תשלומים, מנהל המערכת)</t>
+  </si>
+  <si>
+    <t>קבלת מידע על היסטוריית הרכישות שבוצעה בחנות. על ההיסטוריה להיות אדישה לשינויים החלים במערכת כגון הסרת מוצר, שינוי תיאור מוצר, שינוי מחיר מוצר וכו'</t>
+  </si>
+  <si>
+    <t>לא ניתן ליצור אוביקט של המע' ללא פרטי מנהל מערכת והאוביקטים הנדרשים</t>
+  </si>
+  <si>
+    <t>מבחני יחידה/אינטגרציה</t>
+  </si>
+  <si>
+    <t>יציאה מהמע' תבוצע ע"י סגירת ה- client</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+TradingSystemTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+StoreTest
+InventoryTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+BasketTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+ManageInventoryPermissionTest
+SubscriberTest
+StoreTest
+InventoryTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+OwnerPermissionTest
+SubscriberTest</t>
+  </si>
+  <si>
+    <t>בעל-חנות רשאי למנות מנוי של המערכת (שעדין איננו בעל החנות) לבעל -חנות
+נוסף עבור החנות שלו. למנוי שמונה לבעל-חנות חדש יש זכויות של בעל-חנות לגבי מדיניות וניהול החנות</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+OwnerPermissionTest
+SubscriberTest
+RemovePermissionPermissionTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+OwnerPermissionTest
+ManagerPermissionTest
+SubscriberTest
+RemovePermissionPermissionTest</t>
+  </si>
+  <si>
+    <t>בעל-חנות רשאי להסיר מינוי של מנהל-חנות שמונה על ידו בעבר</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+OwnerPermissionTest
+ManagerPermissionTest
+RemovePermissionPermissionTest
+SubscriberTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+OwnerPermissionTest
+ManagerPermissionTest
+ManageInventoryPermissionTest
+NoPermissionPermissionTest
+SubscriberTest</t>
+  </si>
+  <si>
+    <t>בעל חנות יכול לקבל מידע על כל בעלי התפקידים בחנות והרשאותיהם</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+SubscriberTest
+OwnerPermissionTest</t>
+  </si>
+  <si>
+    <t>same as 4.6</t>
+  </si>
+  <si>
+    <t>PaymentSystem.pay</t>
+  </si>
+  <si>
+    <t>DeliverySystem.deliver</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+UserTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+SubscriberTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+AdminPermissionTest
+SubscriberTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+InventoryTest
+StoreTest</t>
+  </si>
+  <si>
+    <t>בעל חנות רשאי להגדיר, לערוך ולקבל מידע אודות סוגי הרכישה וההנחה האפשריים בחנות, ומדיניות הקנייה וההנחה עבור מוצרים בחנות</t>
+  </si>
+  <si>
+    <t>בעל חנות רשאי להסיר מינוי של בעל חנות שמונה על ידו בעבר. הסרת מינוי של בעל חנות גוררת הסרת כל המינויים של בעלי ומנהלי החנות שמונו על ידו</t>
+  </si>
+  <si>
+    <t>בעלי חנות צריכים לקבל התראת זמן-אמת כאשר לקוח קונה מוצר מחנותם, 
+כאשר חנותם נסגרת או נפתחת מחדש, כאשר המינוי שלהם מוסר, 
+ומקרים אחרים בהתאם לדרישות (למשל סוגי קניה שונים).</t>
+  </si>
+  <si>
+    <t>3.c</t>
+  </si>
+  <si>
+    <t>3.d</t>
+  </si>
+  <si>
+    <t>3.e</t>
+  </si>
+  <si>
+    <t>המערכת צריכה להתמודד עם התקפות המנסות לשבש את ההתנהגות התקינה של המערכת (בגרסה 2, הכוונה לשימוש בפרוטוקולי תקשורת מאובטחים HTTPS/WSS)</t>
+  </si>
+  <si>
+    <t>איפיון ומימוש ממשק משתמש נוח</t>
+  </si>
+  <si>
+    <t>ממשק משתמש ייעודי עבור כל סוג משתמש - ביצוע רק פעולות שהמשתמש רשאי לבצע, בהתאם לתפקידו והרשאותיו.</t>
+  </si>
+  <si>
+    <t>המערכת מספקת הסברים על פעולותיה - הצלחות וכשלונות של פעולות במערכת</t>
+  </si>
+  <si>
+    <t>UserAuthentication.computeHash</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+UserAuthenticationTest</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.removeOwner</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+SubscriberConcurrencyTest
+SubscriberTest</t>
+  </si>
+  <si>
+    <t>DiscountPolicyTest
+PurchasePolicyTest</t>
+  </si>
+  <si>
+    <t>purchaseEmptyCart()
+purchaseOneItemFromOneStore()
+purchaseTwoItemsFromDifferentTwoStores()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TradingSystemServiceImpl.allowManagerToUpdateProducts
 TradingSystemServiceImpl.disableManagerFromUpdateProducts
 TradingSystemServiceImpl.allowManagerToEditPolicies
 TradingSystemServiceImpl.disableManagerFromEditPolicies
 TradingSystemServiceImpl.allowManagerToGetHistory
-TradingSystemServiceImpl.disableManagerFromGetHistory</t>
-  </si>
-  <si>
-    <t>validAllowManagerToUpdateProducts()
+TradingSystemServiceImpl.disableManagerFromGetHistory
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TradingSystemServiceImpl.allowManagerToEditPolicies
+TradingSystemServiceImpl.disableManagerFromEditPolicies</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">validAllowManagerToUpdateProducts()
 wrongAllowManagerToUpdateProducts()
 disableManagerFromUpdateProducts()
 disableManagerFromUpdateProductsWithoutPermissionsInStore()
@@ -320,179 +543,92 @@
 validAllowManagerToGetHistory()
 wrongAllowManagerToGetHistory()
 disableManagerFromGetHistory()
-disableManagerFromGetHistoryWithoutPermissionsInStore()</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceImpl.removeManager</t>
-  </si>
-  <si>
-    <t>validRemoveManager()
-wrongRemoveManager()</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceImpl.showStaffInfo</t>
-  </si>
-  <si>
-    <t>showStaffInfo()
-showStaffInfoStoreNotExist()
-showStaffInfoNoPermissions()</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceImpl.getSalesHistoryByStore</t>
-  </si>
-  <si>
-    <t>getSalesHistoryByStore()
-wrongGetSalesHistoryByStore()</t>
-  </si>
-  <si>
-    <t>ביצוע תשלום</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceImpl.purchaseCart</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceImpl.getEventLog
-TradingSystemServiceImpl.getErrorLog</t>
-  </si>
-  <si>
-    <t>getEventLog()
-wrongGetEventLog()
-getErrorLog()
-wrongGetErrorLog()</t>
-  </si>
-  <si>
-    <t>בביצוע</t>
-  </si>
-  <si>
-    <t>אתחול המערכת המבטיח קיום כל הישויות הנדרשות על פי אילוצי הנכונות (למשל מערכת המסחר, מערכת תשלומים, מנהל המערכת)</t>
-  </si>
-  <si>
-    <t>לא בוצע</t>
-  </si>
-  <si>
-    <t>קבלת מידע על היסטוריית הרכישות שבוצעה בחנות. על ההיסטוריה להיות אדישה לשינויים החלים במערכת כגון הסרת מוצר, שינוי תיאור מוצר, שינוי מחיר מוצר וכו'</t>
-  </si>
-  <si>
-    <t>לא ניתן ליצור אוביקט של המע' ללא פרטי מנהל מערכת והאוביקטים הנדרשים</t>
-  </si>
-  <si>
-    <t>מבחני יחידה/אינטגרציה</t>
-  </si>
-  <si>
-    <t>יציאה מהמע' תבוצע ע"י סגירת ה- client</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-TradingSystemTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-StoreTest
-InventoryTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-BasketTest</t>
-  </si>
-  <si>
-    <t>סוגי רכישה והנחה עדיין לא נדרש לממש. יש לממש בדיקות קבלה ובדיקות יחידה</t>
-  </si>
-  <si>
-    <t>מומש; חסר בדיקות יחידה</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-ManageInventoryPermissionTest
-SubscriberTest
-StoreTest
-InventoryTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-OwnerPermissionTest
-SubscriberTest</t>
-  </si>
-  <si>
-    <t>בעל-חנות רשאי למנות מנוי של המערכת (שעדין איננו בעל החנות) לבעל -חנות
-נוסף עבור החנות שלו. למנוי שמונה לבעל-חנות חדש יש זכויות של בעל-חנות לגבי מדיניות וניהול החנות</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-OwnerPermissionTest
-SubscriberTest
-RemovePermissionPermissionTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-OwnerPermissionTest
-ManagerPermissionTest
-SubscriberTest
-RemovePermissionPermissionTest</t>
-  </si>
-  <si>
-    <t>בעל-חנות רשאי להסיר מינוי של מנהל-חנות שמונה על ידו בעבר</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-OwnerPermissionTest
-ManagerPermissionTest
-RemovePermissionPermissionTest
-SubscriberTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-OwnerPermissionTest
-ManagerPermissionTest
-ManageInventoryPermissionTest
-NoPermissionPermissionTest
-SubscriberTest</t>
-  </si>
-  <si>
-    <t>בעל חנות יכול לקבל מידע על כל בעלי התפקידים בחנות והרשאותיהם</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-SubscriberTest
-OwnerPermissionTest</t>
-  </si>
-  <si>
-    <t>TradingSystemServiceTest
-AdminPermissionTest</t>
-  </si>
-  <si>
-    <t>same as 4.6</t>
-  </si>
-  <si>
-    <t>PaymentSystem.pay</t>
-  </si>
-  <si>
-    <t>DeliverySystem.deliver</t>
-  </si>
-  <si>
-    <t>יש לממש ErrorLog ולהשלים בדיקות יחידה. יש להרחיב את בדיקות הקבלה ל- logs</t>
-  </si>
-  <si>
-    <t>יש תשתית לפניה. להוסיף mock למע' התשלומים בבדיקות הקבלה</t>
-  </si>
-  <si>
-    <t>יש תשתית לפניה. להוסיף mock למע' האספקה בבדיקות הקבלה</t>
-  </si>
-  <si>
-    <t>להוסיף טסטים</t>
+disableManagerFromGetHistoryWithoutPermissionsInStore()
+validAllowToEditPurchasesPoliciesByManager()
+validAllowToEditDiscountsPoliciesByManager()
+notValidAllowManagerOrStoreOwnerToEditPurchases()
+notValidAllowManagerOrStoreOwnerToEditDiscounts()
+</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.getStorePolicies
+TradingSystemServiceImpl.assignStorePurchasePolicy
+TradingSystemServiceImpl.removePolicy
+TradingSystemServiceImpl.makeQuantityPolicy
+TradingSystemServiceImpl.makeBasketPurchasePolicy
+TradingSystemServiceImpl.makeTimePolicy
+TradingSystemServiceImpl.andPolicy
+TradingSystemServiceImpl.orPolicy
+TradingSystemServiceImpl.xorPolicy
+TradingSystemServiceImpl.getStoreDiscounts
+TradingSystemServiceImpl.assignStoreDiscountPolicy
+TradingSystemServiceImpl.removeDiscount
+TradingSystemServiceImpl.makeQuantityDiscount
+TradingSystemServiceImpl.makePlusDiscount
+TradingSystemServiceImpl.makeMaxDiscount</t>
+  </si>
+  <si>
+    <t>basketMustHaveLessThen5KgTomatoesPurchasePolicy()
+tomatoCanBePurchasedOnlyAfter10AMPurchasePolicy()
+basketMustHaveLessThen5KgTomatoesAndAtLeast2CornsPurchasePolicy()
+basketCanHave5KgTomatoesOrMoreOnlyIfThereIsAtLeast1CornPurchasePolicy()
+storeDiscountPolicyOf20Percent()
+sub1CategoryDiscountOf50Percent()
+purchaseValueOf50Gives10PercentOnTomatoesDiscountPolicy()
+sub1With5PercentDiscountIfBasketContainsAtLeast5TomatoesAnd2CornsDiscountPolicy()
+sub1With5PercentDiscountIfBasketContainsAtLeast5TomatoesOr2CornsDiscountPolicy()
+ifBasketValueMoreThen50AndContains3TomatoesSo5PercentOnSub1CategoryDiscountPolicy()
+DiscountOf10PercentOnTomatoesOr5PercentOnCornsDependsOnBestForUserDiscountPolicy()
+DiscountOnVegetables5PercentAnd10PercentOnTomatoesDiscountPolicy()</t>
+  </si>
+  <si>
+    <t>validRemoveStoreOwnerByTheOwnerAssignor()
+removeStoreOwnerWithStoreOwnerWhoDidntAssignTheOwner()
+removeStoreOwnerByOwnerOfAnotherStore()
+removeStoreOwnerByManagerOfTheStore()
+removeStoreOwnerRemovesAllTheManagersAndOwnersWithTheRemovedAssignee()</t>
+  </si>
+  <si>
+    <t>getStoreItemsWithKeyWordMistakes()
+getStoreItemsWithItemNameMistakes()
+getStoreItemsWithCategoryMistakes()</t>
+  </si>
+  <si>
+    <t>NotificationsTests</t>
+  </si>
+  <si>
+    <t>לממש websockets, להשלים unit tests ובדיקות קבלה</t>
+  </si>
+  <si>
+    <t>presentation.TradingSystem</t>
+  </si>
+  <si>
+    <t>ssl package</t>
+  </si>
+  <si>
+    <t>להוסיף טסטים (התחלנו מעבר מjunit לtestNG על מנת לתמוך בזה)</t>
+  </si>
+  <si>
+    <t>gui tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notifications package
+TradingSystemServiceImpl.openNewStore
+TradingSystemServiceImpl.login
+TradingSystemServiceImplwriteOpinionOnProduct
+TradingSystemServiceImpl.purchaseCart
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -500,13 +636,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -590,9 +732,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
@@ -619,6 +758,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -903,85 +1045,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="9.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="3"/>
+    <col min="2" max="2" width="9.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.33203125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="60.88671875" style="15" customWidth="1"/>
-    <col min="8" max="8" width="31.88671875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="34.21875" style="3" customWidth="1"/>
-    <col min="10" max="12" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="12.75" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="80.375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="31.875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="34.25" style="3" customWidth="1"/>
+    <col min="10" max="12" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="6">
         <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>11</v>
       </c>
@@ -994,21 +1136,21 @@
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>94</v>
+      <c r="H3" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="6">
         <v>2.2000000000000002</v>
@@ -1019,19 +1161,19 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="16" t="s">
-        <v>94</v>
+      <c r="E4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="6">
         <v>2.2999999999999998</v>
@@ -1042,21 +1184,21 @@
       <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>94</v>
+      <c r="H5" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="6">
         <v>2.4</v>
@@ -1067,21 +1209,21 @@
       <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>94</v>
+      <c r="H6" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="6">
         <v>2.5</v>
@@ -1092,21 +1234,21 @@
       <c r="D7" s="6">
         <v>1</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>95</v>
+      <c r="H7" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="114" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="6">
         <v>2.6</v>
@@ -1117,21 +1259,21 @@
       <c r="D8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>95</v>
+      <c r="H8" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="6">
         <v>2.7</v>
@@ -1142,21 +1284,21 @@
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>96</v>
+      <c r="H9" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="6">
         <v>2.8</v>
@@ -1167,21 +1309,21 @@
       <c r="D10" s="6">
         <v>1</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="16" t="s">
-        <v>96</v>
+      <c r="H10" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="6">
         <v>2.9</v>
@@ -1190,23 +1332,23 @@
         <v>56</v>
       </c>
       <c r="D11" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>18</v>
       </c>
@@ -1219,21 +1361,21 @@
       <c r="D12" s="6">
         <v>1</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>94</v>
+      <c r="H12" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="6">
         <v>3.2</v>
@@ -1244,21 +1386,21 @@
       <c r="D13" s="6">
         <v>1</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="E13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>94</v>
+      <c r="H13" s="15" t="s">
+        <v>91</v>
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="6">
         <v>3.3</v>
@@ -1267,25 +1409,23 @@
         <v>20</v>
       </c>
       <c r="D14" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="6">
         <v>3.7</v>
@@ -1294,25 +1434,23 @@
         <v>21</v>
       </c>
       <c r="D15" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="H15" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
@@ -1325,407 +1463,567 @@
       <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="16" t="s">
+      <c r="E16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>99</v>
+      <c r="H16" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="6">
         <v>4.3</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="14" t="s">
+      <c r="C18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H17" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="6" t="s">
+      <c r="H18" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>103</v>
+      <c r="H19" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="6">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="D20" s="6">
-        <v>1</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>106</v>
+        <v>2</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="6">
-        <v>4.7</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>104</v>
+        <v>4.5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>105</v>
+      <c r="E21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>98</v>
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="228" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="6">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>107</v>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>108</v>
+      <c r="E22" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="19"/>
+      <c r="B24" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="6">
         <v>4.1100000000000003</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="6">
-        <v>1</v>
-      </c>
-      <c r="E23" s="17" t="s">
+      <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="D25" s="6">
+        <v>2</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="6">
+        <v>2</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="6">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="6">
-        <v>1</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="6">
-        <v>6.4</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="6">
-        <v>1</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="6">
+      <c r="B28" s="6">
         <v>7</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="6">
-        <v>1</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B29" s="6">
         <v>8</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="s">
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="6">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="6">
-        <v>1</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="6">
-        <v>4</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="D30" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="6">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H33" s="15"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="19"/>
+      <c r="B34" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="6">
+        <v>2</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H34" s="15"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="19"/>
+      <c r="B35" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="6">
+        <v>2</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A36" s="19"/>
+      <c r="B36" s="6">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A37" s="19"/>
+      <c r="B37" s="6">
         <v>7</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="6">
-        <v>1</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="16" t="s">
+      <c r="D37" s="6">
+        <v>2</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="19"/>
+      <c r="B38" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="6">
+        <v>2</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>113</v>
+      <c r="F38" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A30:A38"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="A16:A25"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added version 3 requirements and status
</commit_message>
<xml_diff>
--- a/Docs/requirements traceability.xlsx
+++ b/Docs/requirements traceability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omrig\Desktop\BGU\semesterD\Workshop on Software Engineering Project\version2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EF8DB7-5BED-4444-B4B7-BE037720ED37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8C6A15-D483-48B3-AD04-7980EC6502B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="615" windowWidth="13830" windowHeight="7170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
   <si>
     <t>מס' דרישה</t>
   </si>
@@ -524,7 +524,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -606,18 +606,129 @@
     <t>ssl package</t>
   </si>
   <si>
-    <t>להוסיף טסטים (התחלנו מעבר מjunit לtestNG על מנת לתמוך בזה)</t>
-  </si>
-  <si>
     <t>gui tests</t>
   </si>
   <si>
-    <t xml:space="preserve">notifications package
+    <t>המערכת צריכה להתמודד עם אובדן תקשורת בין רכיבים, ועם מערכות חיצוניות</t>
+  </si>
+  <si>
+    <t>המערכת צריכה להיות חסינה להתנהגויות לא צפויות של מערכות חיצוניות, כגון.
+כישלון בשליחת בקשה, ממשק לא תואם, אי מענה לבקשה וכו'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המערכת שומרת את מצבה העדכני במסד נתונים חיצוני של נתונים, באופן המאפשר הפרדה בין פעולות לנתונים. ההפרדה מאפשרת שחזור מצב מערכת וניהול יעיל.
+יש לתמוך במסד הנתונים מרוחק </t>
+  </si>
+  <si>
+    <t>persistence package</t>
+  </si>
+  <si>
+    <t>PersistenceTests</t>
+  </si>
+  <si>
+    <t>איתחול המערכת מתבצע עלפי קובץ קונפיגורציה חיצוני המגדיר
+את הפרמטרים לאתחול</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>המע' מאפשרת איתחול במצב המוגדר בקובץ "מצב" חיצוני: לאחר האיתחול המערכת נמצאת במצב המוגדר בקובץ. קובץ מצב מכיל הנחיות לסדרה של סיפורי שימוש וארגומנטים להפעלתם</t>
+  </si>
+  <si>
+    <t>Main, config.java</t>
+  </si>
+  <si>
+    <t>ConfigurationTests</t>
+  </si>
+  <si>
+    <t>Main, config.script</t>
+  </si>
+  <si>
+    <t>InitialStateTests</t>
+  </si>
+  <si>
+    <t>2.c</t>
+  </si>
+  <si>
+    <t>המערכת תומכת בסוג הקניה הגשת הצעת-קנייה</t>
+  </si>
+  <si>
+    <t>TradingSystemSeviceImpl.addItemToBasketByOffer
+TradingSystemSeviceImpl.getOfferByStore
+TradingSystemSeviceImpl.approveOffer</t>
+  </si>
+  <si>
+    <t>AcceptanceTestsV3:
+add_item_to_basket_by_offer_with_guest
+add_item_to_basket_by_offer_with_subscriber
+get_store_offers_by_guest
+get_store_offers_by_owner_or_manager_without_permission
+get_store_offers_by_owner_with_permission
+approve_offer_by_guest
+approve_offer_by_owner_or_manager_without_permission</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTests
+SubscriberTests
+StoreTests</t>
+  </si>
+  <si>
+    <t>2.d.i</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.getTotalIncomeByStorePerDay</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceImpl.getTotalIncomeByAdminPerDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> מנהל המערכת יכול לצפות בהכנסה הכוללת של המערכת בחתך יומי</t>
+  </si>
+  <si>
+    <t>AcceptanceTestsV3</t>
+  </si>
+  <si>
+    <t>2.d.ii</t>
+  </si>
+  <si>
+    <t>בעלי חנות יכולים לצפות בהכנסות הכוללות של חנותם בחתך יומי</t>
+  </si>
+  <si>
+    <t>SubscriberTests
+OwnerPermissionTests
+TradingSystemServiceTests</t>
+  </si>
+  <si>
+    <t>SubscriberTests
+AdminPermissionTests
+TradingSystemServiceTests</t>
+  </si>
+  <si>
+    <t>TradingSystemServiceTest
+CreateManyStoresWithTheSameNameStressTest
+GiveManagerPermissionByOtherOwners
+PurchaseLastItemByDifferentUsers
+PurchaseRemovedItemFromStore</t>
+  </si>
+  <si>
+    <t>9.1.i</t>
+  </si>
+  <si>
+    <t>התראות למנויים שאינם מחוברים למערכת בזמן ההתראה, נשמרות במערכת ומוצגות להם בביקורם הבא</t>
+  </si>
+  <si>
+    <t>notifications package
 TradingSystemServiceImpl.openNewStore
 TradingSystemServiceImpl.login
 TradingSystemServiceImplwriteOpinionOnProduct
-TradingSystemServiceImpl.purchaseCart
-</t>
+TradingSystemServiceImpl.purchaseCart</t>
+  </si>
+  <si>
+    <t>notifications package</t>
   </si>
 </sst>
 </file>
@@ -628,7 +739,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -636,19 +747,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -679,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -702,11 +813,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="2"/>
@@ -764,6 +912,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,27 +1208,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="3"/>
-    <col min="2" max="2" width="9.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="80.375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="31.875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="34.25" style="3" customWidth="1"/>
-    <col min="10" max="12" width="8.875" style="1"/>
+    <col min="5" max="5" width="12.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.33203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="80.33203125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="34.21875" style="3" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -1094,8 +1259,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="6">
@@ -1123,63 +1288,61 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="22"/>
+      <c r="B3" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B5" s="6">
         <v>2.1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1188,23 +1351,23 @@
         <v>33</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>91</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -1212,24 +1375,22 @@
       <c r="E6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="I6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
       <c r="B7" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -1237,24 +1398,24 @@
       <c r="E7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>51</v>
+      <c r="F7" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="114" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="6">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -1263,23 +1424,23 @@
         <v>33</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="6">
-        <v>2.7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>2.5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1287,24 +1448,24 @@
       <c r="E9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>55</v>
+      <c r="F9" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="6">
-        <v>2.8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>2.6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1312,51 +1473,49 @@
       <c r="E10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>58</v>
+      <c r="F10" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="6">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>18</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
       <c r="B12" s="6">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -1364,126 +1523,126 @@
       <c r="E12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>60</v>
+      <c r="F12" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="22"/>
+      <c r="B15" s="6">
         <v>3.2</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="E15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="6">
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="6">
         <v>3.3</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D16" s="6">
         <v>2</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="13" t="s">
+      <c r="E16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G16" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H16" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="6">
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="6">
         <v>3.7</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D15" s="6">
-        <v>2</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="6">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="6">
-        <v>4.2</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="D17" s="6">
         <v>2</v>
@@ -1491,49 +1650,51 @@
       <c r="E17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>130</v>
+      <c r="F17" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="6">
-        <v>4.3</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>96</v>
+    <row r="18" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
+      <c r="B18" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="D18" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>70</v>
+      <c r="F18" s="15" t="s">
+        <v>153</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="6" t="s">
-        <v>24</v>
+    <row r="19" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="6">
+        <v>4.0999999999999996</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -1541,24 +1702,24 @@
       <c r="E19" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>70</v>
+      <c r="F19" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
+    <row r="20" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
       <c r="B20" s="6">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D20" s="6">
         <v>2</v>
@@ -1566,24 +1727,24 @@
       <c r="E20" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>123</v>
+      <c r="F20" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
       <c r="B21" s="6">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1592,23 +1753,23 @@
         <v>33</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="228" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="6">
-        <v>4.5999999999999996</v>
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
@@ -1616,49 +1777,49 @@
       <c r="E22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>127</v>
+      <c r="F22" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
+    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
       <c r="B23" s="6">
-        <v>4.7</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>99</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="D23" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
+    <row r="24" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
       <c r="B24" s="6">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>102</v>
+        <v>4.5</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -1667,50 +1828,48 @@
         <v>33</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
+    <row r="25" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
       <c r="B25" s="6">
-        <v>4.1100000000000003</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="D25" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="13" t="s">
-        <v>78</v>
+      <c r="F25" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>26</v>
-      </c>
+    <row r="26" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
       <c r="B26" s="6">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>4.7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
@@ -1719,125 +1878,127 @@
         <v>33</v>
       </c>
       <c r="F26" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
+      <c r="B28" s="6">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="6">
+        <v>3</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H30" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B31" s="6">
         <v>6.4</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D27" s="6">
-        <v>2</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="6">
-        <v>7</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="6">
-        <v>8</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="6">
-        <v>1</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="6">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="6">
-        <v>2</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="6">
-        <v>2</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="D31" s="6">
         <v>2</v>
@@ -1846,90 +2007,100 @@
         <v>33</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+        <v>66</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="19"/>
+    <row r="32" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
       <c r="B32" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>31</v>
+        <v>156</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="D32" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>53</v>
+        <v>158</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>110</v>
+        <v>164</v>
       </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="8" t="s">
-        <v>114</v>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="6">
+        <v>7</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="D33" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H33" s="15"/>
+      <c r="F33" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="19"/>
-      <c r="B34" s="8" t="s">
-        <v>115</v>
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="6">
+        <v>8</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D34" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H34" s="15"/>
+      <c r="F34" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="19"/>
-      <c r="B35" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>120</v>
+    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="D35" s="6">
         <v>2</v>
@@ -1937,44 +2108,43 @@
       <c r="E35" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="H35" s="15"/>
+      <c r="F35" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="24" t="s">
+        <v>122</v>
+      </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="6">
-        <v>4</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D36" s="6">
-        <v>1</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
-      <c r="B37" s="6">
-        <v>7</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>8</v>
+      <c r="B37" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="D37" s="6">
         <v>2</v>
@@ -1982,48 +2152,251 @@
       <c r="E37" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>90</v>
+      <c r="F37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
-      <c r="B38" s="6">
-        <v>9.1</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>113</v>
+      <c r="B38" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="D38" s="6">
         <v>2</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="19"/>
+      <c r="B39" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="6">
+        <v>2</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="24"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="19"/>
+      <c r="B40" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="6">
+        <v>2</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" s="24"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="19"/>
+      <c r="B41" s="6">
+        <v>4</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="19"/>
+      <c r="B42" s="6">
+        <v>7</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="6">
+        <v>2</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="6">
+        <v>2</v>
+      </c>
+      <c r="E43" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F43" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" s="24"/>
+      <c r="H43" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="19"/>
+      <c r="B44" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" s="6">
+        <v>2</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="G44" s="24"/>
+      <c r="H44" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="19"/>
+      <c r="B45" s="8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="6">
+        <v>3</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="19"/>
+      <c r="B46" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>134</v>
-      </c>
+      <c r="D46" s="6">
+        <v>3</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="6">
+        <v>6</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="6">
+        <v>3</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I47" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A25"/>
+  <mergeCells count="6">
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A35:A47"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A19:A29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>